<commit_message>
adding bioassay 2 PAM results
</commit_message>
<xml_diff>
--- a/data/2023-06-08_bioassay_2.xlsx
+++ b/data/2023-06-08_bioassay_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Dropbox\PC\Desktop\MS Thesis\MS_Thesis_2023-2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86ADC70-8F1A-49D2-BB22-6D50E8ADE381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F30BC62-7583-48FC-8A75-1A6CE12FA2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{5CCCB351-C044-4070-A66C-061B35931ADB}"/>
+    <workbookView xWindow="11016" yWindow="84" windowWidth="11496" windowHeight="12024" firstSheet="5" activeTab="7" xr2:uid="{5CCCB351-C044-4070-A66C-061B35931ADB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chl" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="NH4" sheetId="7" r:id="rId5"/>
     <sheet name="All Nutrients" sheetId="5" r:id="rId6"/>
     <sheet name="All Nutrients zeroes" sheetId="6" r:id="rId7"/>
+    <sheet name="PAM" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -716,7 +717,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="108">
   <si>
     <t>Number</t>
   </si>
@@ -1038,6 +1039,9 @@
   <si>
     <t>DIN:DIP</t>
   </si>
+  <si>
+    <t>FvFm</t>
+  </si>
 </sst>
 </file>
 
@@ -1175,7 +1179,7 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8742,7 +8746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D503721-5177-475D-B124-D41F3E74F654}">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U1" activeCellId="2" sqref="Q1:Q1048576 S1:S1048576 U1:U1048576"/>
     </sheetView>
   </sheetViews>
@@ -9075,7 +9079,7 @@
         <f t="shared" si="7"/>
         <v>0.52908340120849351</v>
       </c>
-      <c r="U6" s="14" t="e">
+      <c r="U6" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -9132,7 +9136,7 @@
         <f t="shared" si="7"/>
         <v>1.8644697213645747</v>
       </c>
-      <c r="U7" s="14" t="e">
+      <c r="U7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -9189,7 +9193,7 @@
         <f t="shared" si="7"/>
         <v>0.35841778266058</v>
       </c>
-      <c r="U8" s="14" t="e">
+      <c r="U8" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -9246,7 +9250,7 @@
         <f t="shared" si="7"/>
         <v>1.8528772753963592</v>
       </c>
-      <c r="U9" s="14" t="e">
+      <c r="U9" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -9531,7 +9535,7 @@
         <f t="shared" si="7"/>
         <v>0.1435483870967742</v>
       </c>
-      <c r="U14" s="14">
+      <c r="U14">
         <f t="shared" si="8"/>
         <v>0.16625354051927616</v>
       </c>
@@ -9588,7 +9592,7 @@
         <f t="shared" si="7"/>
         <v>4.3684579394995549</v>
       </c>
-      <c r="U15" s="14">
+      <c r="U15">
         <f t="shared" si="8"/>
         <v>5.8432739509052505</v>
       </c>
@@ -9645,7 +9649,7 @@
         <f t="shared" si="7"/>
         <v>1.800911105639005</v>
       </c>
-      <c r="U16" s="14">
+      <c r="U16">
         <f t="shared" si="8"/>
         <v>2.0857625329577596</v>
       </c>
@@ -9702,7 +9706,7 @@
         <f t="shared" si="7"/>
         <v>0.25483870967741939</v>
       </c>
-      <c r="U17" s="14">
+      <c r="U17">
         <f t="shared" si="8"/>
         <v>0.36122436206066444</v>
       </c>
@@ -9987,7 +9991,7 @@
         <f t="shared" si="7"/>
         <v>0.15483870967741933</v>
       </c>
-      <c r="U22" s="14">
+      <c r="U22">
         <f t="shared" si="8"/>
         <v>0.27231541218637989</v>
       </c>
@@ -10044,7 +10048,7 @@
         <f t="shared" si="7"/>
         <v>0.15483870967741936</v>
       </c>
-      <c r="U23" s="14">
+      <c r="U23">
         <f t="shared" si="8"/>
         <v>0.27745343883140594</v>
       </c>
@@ -10101,7 +10105,7 @@
         <f t="shared" si="7"/>
         <v>0.15</v>
       </c>
-      <c r="U24" s="14">
+      <c r="U24">
         <f t="shared" si="8"/>
         <v>0.24144915254237287</v>
       </c>
@@ -10158,7 +10162,7 @@
         <f t="shared" si="7"/>
         <v>0.14032258064516129</v>
       </c>
-      <c r="U25" s="14">
+      <c r="U25">
         <f t="shared" si="8"/>
         <v>0.20822555443548385</v>
       </c>
@@ -10476,4 +10480,634 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24559138-EF72-469B-BA09-14C8956AF8DC}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14">
+        <v>45083</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14">
+        <v>45083</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>0.58499999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14">
+        <v>45083</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>0.63500000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>45083</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>0.57799999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
+        <v>45083</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0.54500000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>0.57399999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>0.67300000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>0.58499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>0.57799999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>0.61699999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>0.72599999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>0.59399999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>0.57399999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>0.72699999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30">
+        <v>0.84899999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>0.68899999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>0.69199999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="14">
+        <v>45085</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>